<commit_message>
-Ganzer Code Eingerückt -Variabelnnamen verbessert
</commit_message>
<xml_diff>
--- a/doc/Variabel-Liste.xlsx
+++ b/doc/Variabel-Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projekt-BLJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C22B3D1-139B-4008-81B1-7B480051C59E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130BE60-5E1D-42D3-A552-0BD98F6107A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{75C22724-BA50-4071-9B85-3ABDF3D3CE26}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="17640" xr2:uid="{75C22724-BA50-4071-9B85-3ABDF3D3CE26}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CCB780-7CED-4D49-87F0-FC5FE8EB8B0C}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>